<commit_message>
etl code and postgre connection
</commit_message>
<xml_diff>
--- a/models/Data Modeling.xlsx
+++ b/models/Data Modeling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabisanches/Desktop/CIS9440 - Data Warehouse/Homework/Homework_GabrieleSanches_CIS9440/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEA5559-FE95-BE47-BB84-6DA97236729B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7660180D-4435-F244-A514-FD9B93FC6A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="540" windowWidth="28040" windowHeight="16460" xr2:uid="{B850F194-FCC4-824B-8C2B-70C24DCF1AE3}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="28040" windowHeight="16460" xr2:uid="{B850F194-FCC4-824B-8C2B-70C24DCF1AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,10 @@
     <author>tc={D2E01190-F4BF-504F-BA44-581FF13B8BFF}</author>
     <author>tc={6F98E277-2CFC-A747-A253-594A23808499}</author>
     <author>tc={65320AEB-DED4-9D4D-81C3-7CEB939E1571}</author>
-    <author>tc={6EA55A50-6F76-FB40-97CE-152BF664175A}</author>
     <author>tc={D7D7C508-A746-5845-8F8E-3AD6A11146E2}</author>
     <author>tc={6D9A9383-4CB5-A74D-B66E-0B9AEB581F4A}</author>
     <author>tc={0743745A-46B8-BD41-8C51-7653B459974F}</author>
     <author>tc={AB370F7B-BA9A-9547-9D0A-0899DB30910C}</author>
-    <author>tc={E28E3E69-FC14-EF45-97E2-461593CCF661}</author>
     <author>tc={CAB75ED5-ED85-C645-BA51-8543EE75F434}</author>
     <author>tc={D3B5311A-F1D6-A143-A68C-772B3BEB0059}</author>
   </authors>
@@ -76,7 +74,7 @@
     Foreign key</t>
       </text>
     </comment>
-    <comment ref="I15" authorId="3" shapeId="0" xr:uid="{6EA55A50-6F76-FB40-97CE-152BF664175A}">
+    <comment ref="I15" authorId="3" shapeId="0" xr:uid="{D7D7C508-A746-5845-8F8E-3AD6A11146E2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -84,7 +82,7 @@
     Foreign key</t>
       </text>
     </comment>
-    <comment ref="I16" authorId="4" shapeId="0" xr:uid="{D7D7C508-A746-5845-8F8E-3AD6A11146E2}">
+    <comment ref="I16" authorId="4" shapeId="0" xr:uid="{6D9A9383-4CB5-A74D-B66E-0B9AEB581F4A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -92,15 +90,7 @@
     Foreign key</t>
       </text>
     </comment>
-    <comment ref="I17" authorId="5" shapeId="0" xr:uid="{6D9A9383-4CB5-A74D-B66E-0B9AEB581F4A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Foreign key</t>
-      </text>
-    </comment>
-    <comment ref="J21" authorId="6" shapeId="0" xr:uid="{0743745A-46B8-BD41-8C51-7653B459974F}">
+    <comment ref="J21" authorId="5" shapeId="0" xr:uid="{0743745A-46B8-BD41-8C51-7653B459974F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +98,7 @@
     Primary Key</t>
       </text>
     </comment>
-    <comment ref="K21" authorId="7" shapeId="0" xr:uid="{AB370F7B-BA9A-9547-9D0A-0899DB30910C}">
+    <comment ref="K21" authorId="6" shapeId="0" xr:uid="{AB370F7B-BA9A-9547-9D0A-0899DB30910C}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -117,7 +107,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="L21" authorId="8" shapeId="0" xr:uid="{E28E3E69-FC14-EF45-97E2-461593CCF661}">
+    <comment ref="L21" authorId="7" shapeId="0" xr:uid="{CAB75ED5-ED85-C645-BA51-8543EE75F434}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -125,15 +115,7 @@
     Primary Key</t>
       </text>
     </comment>
-    <comment ref="M21" authorId="9" shapeId="0" xr:uid="{CAB75ED5-ED85-C645-BA51-8543EE75F434}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Primary Key</t>
-      </text>
-    </comment>
-    <comment ref="N21" authorId="10" shapeId="0" xr:uid="{D3B5311A-F1D6-A143-A68C-772B3BEB0059}">
+    <comment ref="M21" authorId="8" shapeId="0" xr:uid="{D3B5311A-F1D6-A143-A68C-772B3BEB0059}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -146,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
   <si>
     <t>Steps:</t>
   </si>
@@ -406,9 +388,6 @@
     <t xml:space="preserve">Location_Dimension </t>
   </si>
   <si>
-    <t>FactID</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -427,12 +406,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
     <t>vehicle_ID</t>
   </si>
   <si>
@@ -445,18 +418,6 @@
     <t>date_id</t>
   </si>
   <si>
-    <t>time_id</t>
-  </si>
-  <si>
-    <t>vahicle_id</t>
-  </si>
-  <si>
-    <t>*when adding the dimension into the schema, for the name ALWAYS do dim_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*** exmaple: dm_location, dim_date, etc. </t>
-  </si>
-  <si>
     <t xml:space="preserve"> to dploy the schema after the data model</t>
   </si>
   <si>
@@ -505,19 +466,40 @@
     <t>week_of_the_month</t>
   </si>
   <si>
-    <t>hour</t>
-  </si>
-  <si>
     <t>week_of the year</t>
   </si>
   <si>
     <t>Victim</t>
   </si>
   <si>
-    <t>VictimID</t>
-  </si>
-  <si>
     <t xml:space="preserve">     - See if the time the crash happened have a correlation with the number of people killed/injured</t>
+  </si>
+  <si>
+    <t>monthNumber</t>
+  </si>
+  <si>
+    <t>dayNumber</t>
+  </si>
+  <si>
+    <t>dayName</t>
+  </si>
+  <si>
+    <t>MonthName</t>
+  </si>
+  <si>
+    <t>hourNumber</t>
+  </si>
+  <si>
+    <t>vehicle_id</t>
+  </si>
+  <si>
+    <t>contributingfactor_id</t>
+  </si>
+  <si>
+    <t>fact_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1039,13 +1021,10 @@
   <threadedComment ref="I14" dT="2024-03-10T22:35:08.34" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{65320AEB-DED4-9D4D-81C3-7CEB939E1571}">
     <text>Foreign key</text>
   </threadedComment>
-  <threadedComment ref="I15" dT="2024-03-10T22:35:17.37" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{6EA55A50-6F76-FB40-97CE-152BF664175A}">
+  <threadedComment ref="I15" dT="2024-03-10T22:35:22.82" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{D7D7C508-A746-5845-8F8E-3AD6A11146E2}">
     <text>Foreign key</text>
   </threadedComment>
-  <threadedComment ref="I16" dT="2024-03-10T22:35:22.82" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{D7D7C508-A746-5845-8F8E-3AD6A11146E2}">
-    <text>Foreign key</text>
-  </threadedComment>
-  <threadedComment ref="I17" dT="2024-03-10T22:35:30.23" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{6D9A9383-4CB5-A74D-B66E-0B9AEB581F4A}">
+  <threadedComment ref="I16" dT="2024-03-10T22:35:30.23" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{6D9A9383-4CB5-A74D-B66E-0B9AEB581F4A}">
     <text>Foreign key</text>
   </threadedComment>
   <threadedComment ref="J21" dT="2024-03-10T22:35:55.27" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{0743745A-46B8-BD41-8C51-7653B459974F}">
@@ -1055,13 +1034,10 @@
     <text xml:space="preserve">Primary Key
 </text>
   </threadedComment>
-  <threadedComment ref="L21" dT="2024-03-10T22:36:08.13" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{E28E3E69-FC14-EF45-97E2-461593CCF661}">
+  <threadedComment ref="L21" dT="2024-03-10T22:36:27.68" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{CAB75ED5-ED85-C645-BA51-8543EE75F434}">
     <text>Primary Key</text>
   </threadedComment>
-  <threadedComment ref="M21" dT="2024-03-10T22:36:27.68" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{CAB75ED5-ED85-C645-BA51-8543EE75F434}">
-    <text>Primary Key</text>
-  </threadedComment>
-  <threadedComment ref="N21" dT="2024-03-10T22:36:38.30" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{D3B5311A-F1D6-A143-A68C-772B3BEB0059}">
+  <threadedComment ref="M21" dT="2024-03-10T22:36:38.30" personId="{8BD59D4D-3515-5641-8D29-E527D4967F8F}" id="{D3B5311A-F1D6-A143-A68C-772B3BEB0059}">
     <text>Primary Key</text>
   </threadedComment>
 </ThreadedComments>
@@ -1069,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D7632B-E534-C84E-AC2E-2654C4DB800E}">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1086,7 +1062,8 @@
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="30.1640625" customWidth="1"/>
     <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1125,7 +1102,7 @@
         <v>38</v>
       </c>
       <c r="T2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -1150,7 +1127,7 @@
         <v>85</v>
       </c>
       <c r="T3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -1175,7 +1152,7 @@
         <v>84</v>
       </c>
       <c r="T4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -1197,10 +1174,10 @@
         <v>14</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="T5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -1227,7 +1204,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>12</v>
@@ -1267,7 +1244,7 @@
       </c>
       <c r="K8" s="18"/>
       <c r="T8" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -1290,7 +1267,7 @@
       </c>
       <c r="K9" s="18"/>
       <c r="T9" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -1309,11 +1286,11 @@
         <v>67</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="K10" s="18"/>
       <c r="T10" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -1333,7 +1310,7 @@
       </c>
       <c r="K11" s="18"/>
       <c r="T11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -1349,11 +1326,11 @@
         <v>69</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="K12" s="18"/>
       <c r="T12" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
@@ -1369,11 +1346,11 @@
         <v>70</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K13" s="18"/>
       <c r="T13" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -1389,11 +1366,11 @@
         <v>71</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K14" s="18"/>
       <c r="T14" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -1409,7 +1386,7 @@
         <v>72</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="K15" s="18"/>
     </row>
@@ -1426,11 +1403,11 @@
         <v>73</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="K16" s="18"/>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" s="16" t="s">
         <v>23</v>
       </c>
@@ -1442,11 +1419,8 @@
       <c r="G17" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I17" s="18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="16" t="s">
         <v>24</v>
       </c>
@@ -1459,7 +1433,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" s="15" t="s">
         <v>25</v>
       </c>
@@ -1472,7 +1446,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="15" t="s">
         <v>26</v>
       </c>
@@ -1485,22 +1459,19 @@
         <v>77</v>
       </c>
       <c r="J20" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="K20" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="K20" s="22" t="s">
-        <v>88</v>
-      </c>
       <c r="L20" s="22" t="s">
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="N20" s="22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="15" t="s">
         <v>27</v>
       </c>
@@ -1513,22 +1484,19 @@
         <v>63</v>
       </c>
       <c r="J21" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="K21" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="K21" s="24" t="s">
-        <v>90</v>
-      </c>
       <c r="L21" s="24" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="M21" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="N21" s="24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="15" t="s">
         <v>28</v>
       </c>
@@ -1544,16 +1512,16 @@
         <v>25</v>
       </c>
       <c r="K22" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="L22" t="s">
+        <v>107</v>
       </c>
       <c r="M22" t="s">
-        <v>114</v>
-      </c>
-      <c r="N22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="15" t="s">
         <v>29</v>
       </c>
@@ -1567,10 +1535,10 @@
         <v>26</v>
       </c>
       <c r="K23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="15" t="s">
         <v>30</v>
       </c>
@@ -1584,10 +1552,10 @@
         <v>10</v>
       </c>
       <c r="K24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C25" s="13" t="s">
         <v>31</v>
       </c>
@@ -1597,14 +1565,17 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
+      <c r="I25" t="s">
+        <v>123</v>
+      </c>
       <c r="J25" t="s">
         <v>11</v>
       </c>
       <c r="K25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C26" s="16" t="s">
         <v>32</v>
       </c>
@@ -1618,10 +1589,10 @@
         <v>30</v>
       </c>
       <c r="K26" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C27" s="13" t="s">
         <v>33</v>
       </c>
@@ -1633,10 +1604,10 @@
         <v>28</v>
       </c>
       <c r="K27" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C28" s="16" t="s">
         <v>34</v>
       </c>
@@ -1648,10 +1619,10 @@
         <v>27</v>
       </c>
       <c r="K28" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C29" s="13" t="s">
         <v>35</v>
       </c>
@@ -1663,7 +1634,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C30" s="16" t="s">
         <v>36</v>
       </c>
@@ -1671,31 +1642,27 @@
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="K30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="K31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L34" t="s">
-        <v>102</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>